<commit_message>
add castanha in dict
</commit_message>
<xml_diff>
--- a/CAIXA_fechado.xlsx
+++ b/CAIXA_fechado.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" tabRatio="500" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="8190" yWindow="2295" windowWidth="13410" windowHeight="10485" tabRatio="500" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" state="visible" r:id="rId1"/>
@@ -522,7 +522,7 @@
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -556,17 +556,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="16" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="17" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="17" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="17" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="19" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="165" fontId="8" fillId="6" borderId="20" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="right"/>
@@ -577,7 +566,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="17" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="17" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="21" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -597,30 +585,15 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="24" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="6" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="25" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="18" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="165" fontId="8" fillId="0" borderId="20" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="15" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="165" fontId="8" fillId="6" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="20" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="20" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="6" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="165" fontId="8" fillId="6" borderId="24" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
@@ -631,8 +604,28 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="25" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="18" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="15" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="166" fontId="8" fillId="0" borderId="31" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
@@ -1015,10 +1008,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G65"/>
+  <dimension ref="A1:G66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C65" sqref="C65"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" zeroHeight="1"/>
@@ -1034,26 +1027,26 @@
   </cols>
   <sheetData>
     <row r="1" ht="19.5" customHeight="1" thickBot="1">
-      <c r="A1" s="63" t="inlineStr">
+      <c r="A1" s="55" t="inlineStr">
         <is>
           <t>CAIXA DIA //</t>
         </is>
       </c>
-      <c r="B1" s="62" t="n"/>
-      <c r="C1" s="62" t="n"/>
-      <c r="D1" s="62" t="n"/>
-      <c r="E1" s="62" t="n"/>
-      <c r="F1" s="62" t="n"/>
-      <c r="G1" s="28" t="n"/>
+      <c r="B1" s="56" t="n"/>
+      <c r="C1" s="56" t="n"/>
+      <c r="D1" s="56" t="n"/>
+      <c r="E1" s="56" t="n"/>
+      <c r="F1" s="56" t="n"/>
+      <c r="G1" s="54" t="n"/>
     </row>
     <row r="2" ht="4.5" customHeight="1">
-      <c r="A2" s="57" t="n"/>
-      <c r="B2" s="57" t="n"/>
-      <c r="C2" s="58" t="n"/>
-      <c r="D2" s="59" t="n"/>
-      <c r="E2" s="60" t="inlineStr"/>
-      <c r="F2" s="61" t="n"/>
-      <c r="G2" s="61" t="n"/>
+      <c r="A2" s="46" t="n"/>
+      <c r="B2" s="46" t="n"/>
+      <c r="C2" s="47" t="n"/>
+      <c r="D2" s="48" t="n"/>
+      <c r="E2" s="49" t="inlineStr"/>
+      <c r="F2" s="50" t="n"/>
+      <c r="G2" s="50" t="n"/>
     </row>
     <row r="3" ht="23.45" customHeight="1">
       <c r="A3" s="1" t="inlineStr">
@@ -1096,7 +1089,7 @@
       <c r="B4" s="3" t="n">
         <v>36</v>
       </c>
-      <c r="C4" s="64" t="n">
+      <c r="C4" s="61" t="n">
         <v>209.98</v>
       </c>
       <c r="D4" s="4" t="n"/>
@@ -1106,7 +1099,7 @@
         </is>
       </c>
       <c r="F4" s="5" t="n"/>
-      <c r="G4" s="64" t="n"/>
+      <c r="G4" s="61" t="n"/>
     </row>
     <row r="5" ht="21" customHeight="1">
       <c r="A5" s="6" t="inlineStr">
@@ -1117,7 +1110,7 @@
       <c r="B5" s="3" t="n">
         <v>18</v>
       </c>
-      <c r="C5" s="64" t="n">
+      <c r="C5" s="61" t="n">
         <v>102</v>
       </c>
       <c r="D5" s="4" t="n"/>
@@ -1127,7 +1120,7 @@
         </is>
       </c>
       <c r="F5" s="5" t="n"/>
-      <c r="G5" s="64" t="n"/>
+      <c r="G5" s="61" t="n"/>
     </row>
     <row r="6" ht="20.1" customHeight="1">
       <c r="A6" s="6" t="inlineStr">
@@ -1138,7 +1131,7 @@
       <c r="B6" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="C6" s="64" t="n">
+      <c r="C6" s="61" t="n">
         <v>174.02</v>
       </c>
       <c r="D6" s="4" t="n"/>
@@ -1148,7 +1141,7 @@
         </is>
       </c>
       <c r="F6" s="2" t="n"/>
-      <c r="G6" s="64" t="n"/>
+      <c r="G6" s="61" t="n"/>
     </row>
     <row r="7" ht="20.1" customHeight="1">
       <c r="A7" s="6" t="inlineStr">
@@ -1159,7 +1152,7 @@
       <c r="B7" s="3" t="n">
         <v>9</v>
       </c>
-      <c r="C7" s="64" t="n">
+      <c r="C7" s="61" t="n">
         <v>53.72</v>
       </c>
       <c r="D7" s="4" t="n"/>
@@ -1171,7 +1164,7 @@
       <c r="F7" s="3" t="n">
         <v>10</v>
       </c>
-      <c r="G7" s="64" t="n">
+      <c r="G7" s="61" t="n">
         <v>1320</v>
       </c>
     </row>
@@ -1184,7 +1177,7 @@
       <c r="B8" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="C8" s="64" t="n">
+      <c r="C8" s="61" t="n">
         <v>18</v>
       </c>
       <c r="D8" s="4" t="n"/>
@@ -1196,7 +1189,7 @@
       <c r="F8" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="G8" s="64" t="n">
+      <c r="G8" s="61" t="n">
         <v>396</v>
       </c>
     </row>
@@ -1209,7 +1202,7 @@
       <c r="B9" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="C9" s="64" t="n">
+      <c r="C9" s="61" t="n">
         <v>12</v>
       </c>
       <c r="D9" s="4" t="n"/>
@@ -1221,7 +1214,7 @@
       <c r="F9" s="3" t="n">
         <v>19</v>
       </c>
-      <c r="G9" s="64" t="n">
+      <c r="G9" s="61" t="n">
         <v>1710</v>
       </c>
     </row>
@@ -1232,17 +1225,17 @@
         </is>
       </c>
       <c r="B10" s="3" t="n"/>
-      <c r="C10" s="64" t="n"/>
+      <c r="C10" s="61" t="n"/>
       <c r="D10" s="4" t="n"/>
-      <c r="E10" s="42" t="inlineStr">
+      <c r="E10" s="36" t="inlineStr">
         <is>
           <t>MISTA</t>
         </is>
       </c>
-      <c r="F10" s="42" t="n">
+      <c r="F10" s="36" t="n">
         <v>2</v>
       </c>
-      <c r="G10" s="64" t="n">
+      <c r="G10" s="61" t="n">
         <v>263.08</v>
       </c>
     </row>
@@ -1255,20 +1248,20 @@
       <c r="B11" s="3" t="n">
         <v>13</v>
       </c>
-      <c r="C11" s="64" t="n">
+      <c r="C11" s="61" t="n">
         <v>103.93</v>
       </c>
       <c r="D11" s="4" t="n"/>
-      <c r="E11" s="55" t="inlineStr">
+      <c r="E11" s="44" t="inlineStr">
         <is>
           <t>total CAIXAS</t>
         </is>
       </c>
-      <c r="F11" s="65">
+      <c r="F11" s="62">
         <f>SUM(F4:F10)</f>
         <v/>
       </c>
-      <c r="G11" s="65">
+      <c r="G11" s="62">
         <f>SUM(G4:G10)</f>
         <v/>
       </c>
@@ -1282,7 +1275,7 @@
       <c r="B12" s="3" t="n">
         <v>14</v>
       </c>
-      <c r="C12" s="64" t="n">
+      <c r="C12" s="61" t="n">
         <v>140</v>
       </c>
       <c r="D12" s="4" t="n"/>
@@ -1296,7 +1289,7 @@
       <c r="B13" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="C13" s="64" t="n">
+      <c r="C13" s="61" t="n">
         <v>10</v>
       </c>
       <c r="D13" s="4" t="n"/>
@@ -1310,7 +1303,7 @@
       <c r="B14" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="C14" s="64" t="n">
+      <c r="C14" s="61" t="n">
         <v>30</v>
       </c>
       <c r="D14" s="4" t="n"/>
@@ -1322,7 +1315,7 @@
         </is>
       </c>
       <c r="B15" s="3" t="n"/>
-      <c r="C15" s="64" t="n"/>
+      <c r="C15" s="61" t="n"/>
       <c r="D15" s="4" t="n"/>
     </row>
     <row r="16" ht="20.1" customHeight="1">
@@ -1334,7 +1327,7 @@
       <c r="B16" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="C16" s="64" t="n">
+      <c r="C16" s="61" t="n">
         <v>2</v>
       </c>
       <c r="D16" s="4" t="n"/>
@@ -1348,7 +1341,7 @@
       <c r="B17" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="C17" s="64" t="n">
+      <c r="C17" s="61" t="n">
         <v>24.5</v>
       </c>
       <c r="D17" s="4" t="n"/>
@@ -1360,7 +1353,7 @@
         </is>
       </c>
       <c r="B18" s="3" t="n"/>
-      <c r="C18" s="64" t="n"/>
+      <c r="C18" s="61" t="n"/>
       <c r="D18" s="4" t="n"/>
     </row>
     <row r="19" ht="20.1" customHeight="1">
@@ -1370,148 +1363,143 @@
         </is>
       </c>
       <c r="B19" s="3" t="n"/>
-      <c r="C19" s="64" t="n"/>
+      <c r="C19" s="61" t="n"/>
       <c r="D19" s="4" t="n"/>
     </row>
     <row r="20" ht="20.1" customHeight="1">
-      <c r="A20" s="6" t="inlineStr">
-        <is>
-          <t>nego bom</t>
-        </is>
-      </c>
-      <c r="B20" s="3" t="n">
-        <v>4</v>
-      </c>
-      <c r="C20" s="64" t="n">
-        <v>40</v>
-      </c>
+      <c r="A20" s="23" t="inlineStr">
+        <is>
+          <t>castanha</t>
+        </is>
+      </c>
+      <c r="B20" s="24" t="n"/>
+      <c r="C20" s="61" t="n"/>
       <c r="D20" s="4" t="n"/>
     </row>
     <row r="21" ht="20.1" customHeight="1">
       <c r="A21" s="6" t="inlineStr">
         <is>
-          <t>pé de moça</t>
-        </is>
-      </c>
-      <c r="B21" s="3" t="n"/>
-      <c r="C21" s="64" t="n"/>
+          <t>nego bom</t>
+        </is>
+      </c>
+      <c r="B21" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="C21" s="61" t="n">
+        <v>40</v>
+      </c>
       <c r="D21" s="4" t="n"/>
     </row>
     <row r="22" ht="20.1" customHeight="1">
       <c r="A22" s="6" t="inlineStr">
         <is>
-          <t>beiju recheado</t>
-        </is>
-      </c>
-      <c r="B22" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="C22" s="64" t="n">
-        <v>12</v>
-      </c>
+          <t>pé de moça</t>
+        </is>
+      </c>
+      <c r="B22" s="3" t="n"/>
+      <c r="C22" s="61" t="n"/>
       <c r="D22" s="4" t="n"/>
     </row>
     <row r="23" ht="20.1" customHeight="1">
       <c r="A23" s="6" t="inlineStr">
         <is>
-          <t>biscoito alexandre</t>
+          <t>beiju recheado</t>
         </is>
       </c>
       <c r="B23" s="3" t="n">
-        <v>4</v>
-      </c>
-      <c r="C23" s="64" t="n">
-        <v>59.28</v>
+        <v>1</v>
+      </c>
+      <c r="C23" s="61" t="n">
+        <v>12</v>
       </c>
       <c r="D23" s="4" t="n"/>
     </row>
     <row r="24" ht="20.1" customHeight="1">
       <c r="A24" s="6" t="inlineStr">
         <is>
-          <t>brigadeiro</t>
+          <t>biscoito alexandre</t>
         </is>
       </c>
       <c r="B24" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="C24" s="64" t="n">
-        <v>7</v>
+        <v>4</v>
+      </c>
+      <c r="C24" s="61" t="n">
+        <v>59.28</v>
       </c>
       <c r="D24" s="4" t="n"/>
     </row>
     <row r="25" ht="20.1" customHeight="1">
       <c r="A25" s="6" t="inlineStr">
         <is>
-          <t>pingo bel</t>
+          <t>brigadeiro</t>
         </is>
       </c>
       <c r="B25" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="C25" s="64" t="n">
-        <v>3.5</v>
+        <v>2</v>
+      </c>
+      <c r="C25" s="61" t="n">
+        <v>7</v>
       </c>
       <c r="D25" s="4" t="n"/>
     </row>
     <row r="26" ht="20.1" customHeight="1">
       <c r="A26" s="6" t="inlineStr">
         <is>
-          <t>frigelis preta</t>
-        </is>
-      </c>
-      <c r="B26" s="3" t="n"/>
-      <c r="C26" s="64" t="n"/>
+          <t>pingo bel</t>
+        </is>
+      </c>
+      <c r="B26" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C26" s="61" t="n">
+        <v>3.5</v>
+      </c>
       <c r="D26" s="4" t="n"/>
-      <c r="E26" s="22" t="n"/>
     </row>
     <row r="27" ht="20.1" customHeight="1">
       <c r="A27" s="6" t="inlineStr">
         <is>
-          <t>frigelis verde</t>
+          <t>frigelis preta</t>
         </is>
       </c>
       <c r="B27" s="3" t="n"/>
-      <c r="C27" s="64" t="n"/>
+      <c r="C27" s="61" t="n"/>
       <c r="D27" s="4" t="n"/>
       <c r="E27" s="22" t="n"/>
     </row>
     <row r="28" ht="20.1" customHeight="1">
-      <c r="A28" s="2" t="inlineStr">
-        <is>
-          <t>frigelis vermelha</t>
+      <c r="A28" s="6" t="inlineStr">
+        <is>
+          <t>frigelis verde</t>
         </is>
       </c>
       <c r="B28" s="3" t="n"/>
-      <c r="C28" s="64" t="n"/>
+      <c r="C28" s="61" t="n"/>
       <c r="D28" s="4" t="n"/>
       <c r="E28" s="22" t="n"/>
     </row>
     <row r="29" ht="20.1" customHeight="1">
-      <c r="A29" s="6" t="inlineStr">
-        <is>
-          <t>cocada grande</t>
-        </is>
-      </c>
-      <c r="B29" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="C29" s="64" t="n">
-        <v>20</v>
-      </c>
+      <c r="A29" s="2" t="inlineStr">
+        <is>
+          <t>frigelis vermelha</t>
+        </is>
+      </c>
+      <c r="B29" s="3" t="n"/>
+      <c r="C29" s="61" t="n"/>
       <c r="D29" s="4" t="n"/>
       <c r="E29" s="22" t="n"/>
     </row>
     <row r="30" ht="20.1" customHeight="1">
       <c r="A30" s="6" t="inlineStr">
         <is>
-          <t>cocada pequena</t>
+          <t>cocada grande</t>
         </is>
       </c>
       <c r="B30" s="3" t="n">
-        <v>4</v>
-      </c>
-      <c r="C30" s="64" t="n">
-        <v>14</v>
+        <v>2</v>
+      </c>
+      <c r="C30" s="61" t="n">
+        <v>20</v>
       </c>
       <c r="D30" s="4" t="n"/>
       <c r="E30" s="22" t="n"/>
@@ -1519,330 +1507,344 @@
     <row r="31" ht="20.1" customHeight="1">
       <c r="A31" s="6" t="inlineStr">
         <is>
-          <t>bala de yogurt</t>
-        </is>
-      </c>
-      <c r="B31" s="3" t="n"/>
-      <c r="C31" s="64" t="n"/>
+          <t>cocada pequena</t>
+        </is>
+      </c>
+      <c r="B31" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="C31" s="61" t="n">
+        <v>14</v>
+      </c>
       <c r="D31" s="4" t="n"/>
       <c r="E31" s="22" t="n"/>
     </row>
     <row r="32" ht="20.1" customHeight="1">
       <c r="A32" s="6" t="inlineStr">
         <is>
-          <t>pirulito</t>
+          <t>bala de yogurt</t>
         </is>
       </c>
       <c r="B32" s="3" t="n"/>
-      <c r="C32" s="64" t="n"/>
+      <c r="C32" s="61" t="n"/>
       <c r="D32" s="4" t="n"/>
       <c r="E32" s="22" t="n"/>
     </row>
     <row r="33" ht="20.1" customHeight="1">
-      <c r="A33" s="34" t="inlineStr">
-        <is>
-          <t>coquero</t>
-        </is>
-      </c>
-      <c r="B33" s="24" t="n"/>
-      <c r="C33" s="64" t="n"/>
+      <c r="A33" s="6" t="inlineStr">
+        <is>
+          <t>pirulito</t>
+        </is>
+      </c>
+      <c r="B33" s="3" t="n"/>
+      <c r="C33" s="61" t="n"/>
       <c r="D33" s="4" t="n"/>
       <c r="E33" s="22" t="n"/>
     </row>
     <row r="34" ht="20.1" customHeight="1">
-      <c r="A34" s="34" t="inlineStr">
-        <is>
-          <t>zambanana</t>
+      <c r="A34" s="23" t="inlineStr">
+        <is>
+          <t>coquero</t>
         </is>
       </c>
       <c r="B34" s="24" t="n"/>
-      <c r="C34" s="64" t="n"/>
+      <c r="C34" s="61" t="n"/>
       <c r="D34" s="4" t="n"/>
       <c r="E34" s="22" t="n"/>
     </row>
     <row r="35" ht="20.1" customHeight="1">
-      <c r="A35" s="6" t="inlineStr">
-        <is>
-          <t>coca</t>
-        </is>
-      </c>
-      <c r="B35" s="3" t="n">
-        <v>3</v>
-      </c>
-      <c r="C35" s="64" t="n">
-        <v>15</v>
-      </c>
+      <c r="A35" s="23" t="inlineStr">
+        <is>
+          <t>zambanana</t>
+        </is>
+      </c>
+      <c r="B35" s="24" t="n"/>
+      <c r="C35" s="61" t="n"/>
       <c r="D35" s="4" t="n"/>
+      <c r="E35" s="22" t="n"/>
     </row>
     <row r="36" ht="20.1" customHeight="1">
       <c r="A36" s="6" t="inlineStr">
         <is>
-          <t>coca zero</t>
-        </is>
-      </c>
-      <c r="B36" s="3" t="n"/>
-      <c r="C36" s="64" t="n"/>
+          <t>coca</t>
+        </is>
+      </c>
+      <c r="B36" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="C36" s="61" t="n">
+        <v>15</v>
+      </c>
       <c r="D36" s="4" t="n"/>
     </row>
     <row r="37" ht="20.1" customHeight="1">
       <c r="A37" s="6" t="inlineStr">
         <is>
-          <t>fanta</t>
+          <t>coca zero</t>
         </is>
       </c>
       <c r="B37" s="3" t="n"/>
-      <c r="C37" s="64" t="n"/>
+      <c r="C37" s="61" t="n"/>
       <c r="D37" s="4" t="n"/>
     </row>
     <row r="38" ht="20.1" customHeight="1">
       <c r="A38" s="6" t="inlineStr">
         <is>
-          <t>sukita</t>
+          <t>fanta</t>
         </is>
       </c>
       <c r="B38" s="3" t="n"/>
-      <c r="C38" s="64" t="n"/>
+      <c r="C38" s="61" t="n"/>
       <c r="D38" s="4" t="n"/>
     </row>
     <row r="39" ht="20.1" customHeight="1">
       <c r="A39" s="6" t="inlineStr">
         <is>
+          <t>sukita</t>
+        </is>
+      </c>
+      <c r="B39" s="3" t="n"/>
+      <c r="C39" s="61" t="n"/>
+      <c r="D39" s="4" t="n"/>
+    </row>
+    <row r="40" ht="20.1" customHeight="1">
+      <c r="A40" s="6" t="inlineStr">
+        <is>
           <t>guarana</t>
         </is>
       </c>
-      <c r="B39" s="3" t="n"/>
-      <c r="C39" s="64" t="n"/>
-      <c r="D39" s="4" t="n"/>
-    </row>
-    <row r="40" ht="20.1" customHeight="1">
-      <c r="A40" s="34" t="inlineStr">
+      <c r="B40" s="3" t="n"/>
+      <c r="C40" s="61" t="n"/>
+      <c r="D40" s="4" t="n"/>
+    </row>
+    <row r="41" ht="20.1" customHeight="1">
+      <c r="A41" s="23" t="inlineStr">
         <is>
           <t>limoneto</t>
         </is>
       </c>
-      <c r="B40" s="24" t="n"/>
-      <c r="C40" s="64" t="n"/>
-      <c r="D40" s="4" t="n"/>
-    </row>
-    <row r="41" ht="20.1" customHeight="1">
-      <c r="A41" s="6" t="inlineStr">
-        <is>
-          <t>agua</t>
-        </is>
-      </c>
-      <c r="B41" s="3" t="n">
-        <v>4</v>
-      </c>
-      <c r="C41" s="64" t="n">
-        <v>11.99</v>
-      </c>
+      <c r="B41" s="24" t="n"/>
+      <c r="C41" s="61" t="n"/>
       <c r="D41" s="4" t="n"/>
     </row>
     <row r="42" ht="20.1" customHeight="1">
       <c r="A42" s="6" t="inlineStr">
         <is>
-          <t>agua c/ gás</t>
-        </is>
-      </c>
-      <c r="B42" s="3" t="n"/>
-      <c r="C42" s="64" t="n"/>
+          <t>agua</t>
+        </is>
+      </c>
+      <c r="B42" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="C42" s="61" t="n">
+        <v>11.99</v>
+      </c>
       <c r="D42" s="4" t="n"/>
     </row>
     <row r="43" ht="20.1" customHeight="1">
       <c r="A43" s="6" t="inlineStr">
         <is>
+          <t>agua c/ gás</t>
+        </is>
+      </c>
+      <c r="B43" s="3" t="n"/>
+      <c r="C43" s="61" t="n"/>
+      <c r="D43" s="4" t="n"/>
+    </row>
+    <row r="44" ht="20.1" customHeight="1">
+      <c r="A44" s="6" t="inlineStr">
+        <is>
           <t>caixa de presente</t>
         </is>
       </c>
-      <c r="B43" s="3" t="n"/>
-      <c r="C43" s="64" t="n"/>
-      <c r="D43" s="4" t="n"/>
-    </row>
-    <row r="44" ht="20.1" customHeight="1" thickBot="1">
-      <c r="A44" s="41" t="inlineStr">
+      <c r="B44" s="3" t="n"/>
+      <c r="C44" s="61" t="n"/>
+      <c r="D44" s="4" t="n"/>
+    </row>
+    <row r="45" ht="20.1" customHeight="1" thickBot="1">
+      <c r="A45" s="35" t="inlineStr">
         <is>
           <t>estojo bolacha</t>
         </is>
       </c>
-      <c r="B44" s="42" t="n"/>
-      <c r="C44" s="64" t="n"/>
-      <c r="D44" s="7" t="n"/>
-    </row>
-    <row r="45" ht="20.1" customHeight="1" thickBot="1">
-      <c r="A45" s="45" t="inlineStr">
+      <c r="B45" s="36" t="n"/>
+      <c r="C45" s="61" t="n"/>
+      <c r="D45" s="7" t="n"/>
+    </row>
+    <row r="46" ht="20.1" customHeight="1" thickBot="1">
+      <c r="A46" s="39" t="inlineStr">
         <is>
           <t>TOTAL UNIDADES</t>
         </is>
       </c>
-      <c r="B45" s="44">
-        <f>SUM(B3:B44)</f>
+      <c r="B46" s="38">
+        <f>SUM(B3:B45)</f>
         <v/>
       </c>
-      <c r="C45" s="65">
-        <f>SUM(C4:C44)</f>
+      <c r="C46" s="62">
+        <f>SUM(C4:C45)</f>
         <v/>
       </c>
-      <c r="D45" s="7" t="n"/>
-    </row>
-    <row r="46" ht="7.5" customHeight="1" thickBot="1">
-      <c r="A46" s="8" t="n"/>
-      <c r="B46" s="9" t="n"/>
-      <c r="C46" s="10" t="n"/>
       <c r="D46" s="7" t="n"/>
     </row>
-    <row r="47" ht="20.1" customHeight="1" thickBot="1">
-      <c r="A47" s="27" t="inlineStr">
+    <row r="47" ht="7.5" customHeight="1" thickBot="1">
+      <c r="A47" s="8" t="n"/>
+      <c r="B47" s="9" t="n"/>
+      <c r="C47" s="10" t="n"/>
+      <c r="D47" s="7" t="n"/>
+    </row>
+    <row r="48" ht="20.1" customHeight="1" thickBot="1">
+      <c r="A48" s="53" t="inlineStr">
         <is>
           <t>TOTAL de VENDAS</t>
         </is>
       </c>
-      <c r="B47" s="28" t="n"/>
-      <c r="C47" s="65">
-        <f>SUM(G11+C45)</f>
+      <c r="B48" s="54" t="n"/>
+      <c r="C48" s="62">
+        <f>SUM(G11+C46)</f>
         <v/>
       </c>
-      <c r="D47" s="7" t="n"/>
-    </row>
-    <row r="48" ht="9" customHeight="1" thickBot="1">
-      <c r="A48" s="37" t="n"/>
-      <c r="B48" s="38" t="n"/>
-      <c r="C48" s="39" t="n"/>
       <c r="D48" s="7" t="n"/>
     </row>
-    <row r="49" ht="20.1" customHeight="1" thickBot="1">
-      <c r="A49" s="25" t="inlineStr">
+    <row r="49" ht="9" customHeight="1" thickBot="1">
+      <c r="A49" s="31" t="n"/>
+      <c r="B49" s="32" t="n"/>
+      <c r="C49" s="33" t="n"/>
+      <c r="D49" s="7" t="n"/>
+    </row>
+    <row r="50" ht="20.1" customHeight="1" thickBot="1">
+      <c r="A50" s="51" t="inlineStr">
         <is>
           <t>DESPESAS</t>
         </is>
       </c>
-      <c r="B49" s="26" t="n"/>
-      <c r="C49" s="12" t="n"/>
-      <c r="D49" s="7" t="n"/>
-    </row>
-    <row r="50" ht="17.25" customHeight="1">
-      <c r="A50" s="53" t="n"/>
-      <c r="B50" s="64" t="n"/>
-      <c r="C50" s="13" t="n"/>
-    </row>
-    <row r="51" ht="15" customFormat="1" customHeight="1" s="14">
-      <c r="A51" s="32" t="n"/>
-      <c r="B51" s="64" t="n"/>
-    </row>
-    <row r="52" ht="18" customHeight="1">
-      <c r="A52" s="33" t="n"/>
-      <c r="B52" s="64" t="n"/>
-      <c r="C52" s="12" t="n"/>
-    </row>
-    <row r="53" ht="20.1" customHeight="1">
-      <c r="A53" s="34" t="n"/>
-      <c r="B53" s="64" t="n"/>
+      <c r="B50" s="52" t="n"/>
+      <c r="C50" s="12" t="n"/>
+      <c r="D50" s="7" t="n"/>
+    </row>
+    <row r="51" ht="17.25" customHeight="1">
+      <c r="A51" s="43" t="n"/>
+      <c r="B51" s="61" t="n"/>
+      <c r="C51" s="13" t="n"/>
+    </row>
+    <row r="52" ht="15" customFormat="1" customHeight="1" s="14">
+      <c r="A52" s="27" t="n"/>
+      <c r="B52" s="61" t="n"/>
+    </row>
+    <row r="53" ht="18" customHeight="1">
+      <c r="A53" s="28" t="n"/>
+      <c r="B53" s="61" t="n"/>
       <c r="C53" s="12" t="n"/>
     </row>
     <row r="54" ht="20.1" customHeight="1">
-      <c r="A54" s="35" t="n"/>
-      <c r="B54" s="64" t="n"/>
+      <c r="A54" s="23" t="n"/>
+      <c r="B54" s="61" t="n"/>
       <c r="C54" s="12" t="n"/>
     </row>
     <row r="55" ht="20.1" customHeight="1">
-      <c r="A55" s="35" t="n"/>
-      <c r="B55" s="64" t="n"/>
+      <c r="A55" s="29" t="n"/>
+      <c r="B55" s="61" t="n"/>
       <c r="C55" s="12" t="n"/>
     </row>
-    <row r="56" ht="20.1" customHeight="1" thickBot="1">
-      <c r="A56" s="30" t="inlineStr">
+    <row r="56" ht="20.1" customHeight="1">
+      <c r="A56" s="29" t="n"/>
+      <c r="B56" s="61" t="n"/>
+      <c r="C56" s="12" t="n"/>
+    </row>
+    <row r="57" ht="20.1" customHeight="1" thickBot="1">
+      <c r="A57" s="25" t="inlineStr">
         <is>
           <t>TOTAL DESPESAS</t>
         </is>
       </c>
-      <c r="B56" s="65">
-        <f>SUM(B52:B55)</f>
+      <c r="B57" s="62">
+        <f>SUM(B53:B56)</f>
         <v/>
       </c>
-      <c r="C56" s="12" t="n"/>
-    </row>
-    <row r="57" ht="9" customHeight="1" thickBot="1">
-      <c r="A57" s="66" t="n"/>
-      <c r="B57" s="67" t="n"/>
       <c r="C57" s="12" t="n"/>
     </row>
-    <row r="58" ht="18.75" customHeight="1" thickBot="1">
-      <c r="A58" s="68" t="inlineStr">
+    <row r="58" ht="9" customHeight="1" thickBot="1">
+      <c r="A58" s="63" t="n"/>
+      <c r="B58" s="64" t="n"/>
+      <c r="C58" s="12" t="n"/>
+    </row>
+    <row r="59" ht="18.75" customHeight="1" thickBot="1">
+      <c r="A59" s="65" t="inlineStr">
         <is>
           <t>TOTAL/RECEBIDO</t>
         </is>
       </c>
-      <c r="B58" s="26" t="n"/>
-      <c r="C58" s="12" t="n"/>
-    </row>
-    <row r="59" ht="18.75" customFormat="1" customHeight="1" s="16">
-      <c r="A59" s="48" t="inlineStr">
+      <c r="B59" s="52" t="n"/>
+      <c r="C59" s="12" t="n"/>
+    </row>
+    <row r="60" ht="18.75" customFormat="1" customHeight="1" s="16">
+      <c r="A60" s="40" t="inlineStr">
         <is>
           <t>DINHEIRO</t>
         </is>
       </c>
-      <c r="B59" s="64" t="n">
+      <c r="B60" s="61" t="n">
         <v>183</v>
       </c>
-      <c r="C59" s="15" t="n"/>
-    </row>
-    <row r="60" ht="18.75" customHeight="1">
-      <c r="A60" s="17" t="inlineStr">
+      <c r="C60" s="15" t="n"/>
+    </row>
+    <row r="61" ht="18.75" customHeight="1">
+      <c r="A61" s="17" t="inlineStr">
         <is>
           <t>DEBITO</t>
         </is>
       </c>
-      <c r="B60" s="64" t="n">
+      <c r="B61" s="61" t="n">
         <v>182</v>
       </c>
-      <c r="C60" s="12" t="n"/>
-    </row>
-    <row r="61" ht="18.75" customHeight="1">
-      <c r="A61" s="18" t="inlineStr">
+      <c r="C61" s="12" t="n"/>
+    </row>
+    <row r="62" ht="18.75" customHeight="1">
+      <c r="A62" s="18" t="inlineStr">
         <is>
           <t>PIX</t>
         </is>
       </c>
-      <c r="B61" s="64" t="n">
+      <c r="B62" s="61" t="n">
         <v>328</v>
       </c>
-      <c r="C61" s="12" t="n"/>
-    </row>
-    <row r="62" ht="18.75" customHeight="1" thickBot="1">
-      <c r="A62" s="18" t="inlineStr">
+      <c r="C62" s="12" t="n"/>
+    </row>
+    <row r="63" ht="18.75" customHeight="1" thickBot="1">
+      <c r="A63" s="18" t="inlineStr">
         <is>
           <t>PRAZO</t>
         </is>
       </c>
-      <c r="B62" s="64" t="n"/>
-    </row>
-    <row r="63" ht="19.5" customHeight="1" thickBot="1">
-      <c r="A63" s="19" t="inlineStr">
+      <c r="B63" s="61" t="n"/>
+    </row>
+    <row r="64" ht="19.5" customHeight="1" thickBot="1">
+      <c r="A64" s="19" t="inlineStr">
         <is>
           <t>total/recebido</t>
         </is>
       </c>
-      <c r="B63" s="65">
-        <f>SUM(B61+B56+B57+B59+B60+B62)</f>
+      <c r="B64" s="62">
+        <f>SUM(B62+B57+B58+B60+B61+B63)</f>
         <v/>
       </c>
     </row>
-    <row r="64" ht="9" customHeight="1" thickBot="1">
-      <c r="A64" s="20" t="n"/>
-      <c r="B64" s="11" t="n"/>
-    </row>
-    <row r="65" ht="24" customHeight="1" thickBot="1">
-      <c r="A65" s="25" t="inlineStr">
+    <row r="65" ht="9" customHeight="1" thickBot="1">
+      <c r="A65" s="20" t="n"/>
+      <c r="B65" s="11" t="n"/>
+    </row>
+    <row r="66" ht="24" customHeight="1" thickBot="1">
+      <c r="A66" s="51" t="inlineStr">
         <is>
           <t>TOTAL em DINHEIRO</t>
         </is>
       </c>
-      <c r="B65" s="26" t="n"/>
-      <c r="C65" s="65">
-        <f>SUM(B59-B54)</f>
+      <c r="B66" s="52" t="n"/>
+      <c r="C66" s="62">
+        <f>SUM(B60-B55)</f>
         <v/>
       </c>
     </row>
-    <row r="66" ht="15" customHeight="1"/>
     <row r="67" ht="15" customHeight="1"/>
     <row r="68" ht="15" customHeight="1"/>
     <row r="69" ht="15" customHeight="1"/>
@@ -1853,14 +1855,15 @@
     <row r="74" ht="15" customHeight="1"/>
     <row r="75" ht="15" customHeight="1"/>
     <row r="76" ht="15" customHeight="1"/>
+    <row r="77" ht="15" customHeight="1"/>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A48:B48"/>
     <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A65:B65"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="A66:B66"/>
     <mergeCell ref="A58:B58"/>
+    <mergeCell ref="A50:B50"/>
   </mergeCells>
   <pageMargins left="0.511805555555555" right="0.511805555555555" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup orientation="portrait" paperSize="9" firstPageNumber="0" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
recebimentos e sangrias implementados
</commit_message>
<xml_diff>
--- a/CAIXA_fechado.xlsx
+++ b/CAIXA_fechado.xlsx
@@ -959,7 +959,7 @@
     <row r="1" ht="19.5" customHeight="1" s="55">
       <c r="A1" s="56" t="inlineStr">
         <is>
-          <t>CAIXA DIA 12/11/2025</t>
+          <t>CAIXA DIA 15/11/2025</t>
         </is>
       </c>
       <c r="B1" s="57" t="n"/>
@@ -1017,10 +1017,10 @@
         </is>
       </c>
       <c r="B4" s="66" t="n">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C4" s="67" t="n">
-        <v>209.98</v>
+        <v>196.38</v>
       </c>
       <c r="D4" s="68" t="n"/>
       <c r="E4" s="69" t="inlineStr">
@@ -1038,10 +1038,10 @@
         </is>
       </c>
       <c r="B5" s="66" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C5" s="67" t="n">
-        <v>102</v>
+        <v>100.37</v>
       </c>
       <c r="D5" s="68" t="n"/>
       <c r="E5" s="69" t="inlineStr">
@@ -1059,10 +1059,10 @@
         </is>
       </c>
       <c r="B6" s="66" t="n">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="C6" s="67" t="n">
-        <v>174.02</v>
+        <v>101.45</v>
       </c>
       <c r="D6" s="68" t="n"/>
       <c r="E6" s="66" t="inlineStr">
@@ -1080,10 +1080,10 @@
         </is>
       </c>
       <c r="B7" s="66" t="n">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="C7" s="67" t="n">
-        <v>53.72</v>
+        <v>142.63</v>
       </c>
       <c r="D7" s="68" t="n"/>
       <c r="E7" s="66" t="inlineStr">
@@ -1092,10 +1092,10 @@
         </is>
       </c>
       <c r="F7" s="66" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="G7" s="67" t="n">
-        <v>1320</v>
+        <v>264</v>
       </c>
     </row>
     <row r="8" ht="19.5" customHeight="1" s="55">
@@ -1105,10 +1105,10 @@
         </is>
       </c>
       <c r="B8" s="66" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="C8" s="67" t="n">
-        <v>18</v>
+        <v>57.84</v>
       </c>
       <c r="D8" s="68" t="n"/>
       <c r="E8" s="66" t="inlineStr">
@@ -1129,12 +1129,8 @@
           <t>pacote coquinho</t>
         </is>
       </c>
-      <c r="B9" s="66" t="n">
-        <v>2</v>
-      </c>
-      <c r="C9" s="67" t="n">
-        <v>12</v>
-      </c>
+      <c r="B9" s="66" t="n"/>
+      <c r="C9" s="67" t="n"/>
       <c r="D9" s="68" t="n"/>
       <c r="E9" s="66" t="inlineStr">
         <is>
@@ -1142,10 +1138,10 @@
         </is>
       </c>
       <c r="F9" s="66" t="n">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="G9" s="67" t="n">
-        <v>1710</v>
+        <v>535.23</v>
       </c>
     </row>
     <row r="10" ht="19.5" customHeight="1" s="55">
@@ -1154,8 +1150,12 @@
           <t>sequilho</t>
         </is>
       </c>
-      <c r="B10" s="66" t="n"/>
-      <c r="C10" s="67" t="n"/>
+      <c r="B10" s="66" t="n">
+        <v>5</v>
+      </c>
+      <c r="C10" s="67" t="n">
+        <v>14.96</v>
+      </c>
       <c r="D10" s="68" t="n"/>
       <c r="E10" s="71" t="inlineStr">
         <is>
@@ -1163,10 +1163,10 @@
         </is>
       </c>
       <c r="F10" s="71" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G10" s="67" t="n">
-        <v>263.08</v>
+        <v>388.98</v>
       </c>
     </row>
     <row r="11" ht="19.5" customHeight="1" s="55">
@@ -1176,10 +1176,10 @@
         </is>
       </c>
       <c r="B11" s="66" t="n">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C11" s="67" t="n">
-        <v>103.93</v>
+        <v>39.7</v>
       </c>
       <c r="D11" s="68" t="n"/>
       <c r="E11" s="72" t="inlineStr">
@@ -1203,10 +1203,10 @@
         </is>
       </c>
       <c r="B12" s="66" t="n">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="C12" s="67" t="n">
-        <v>140</v>
+        <v>40</v>
       </c>
       <c r="D12" s="68" t="n"/>
     </row>
@@ -1217,10 +1217,10 @@
         </is>
       </c>
       <c r="B13" s="66" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C13" s="67" t="n">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="D13" s="68" t="n"/>
     </row>
@@ -1244,8 +1244,12 @@
           <t>bolo de rolo grande</t>
         </is>
       </c>
-      <c r="B15" s="66" t="n"/>
-      <c r="C15" s="67" t="n"/>
+      <c r="B15" s="66" t="n">
+        <v>1</v>
+      </c>
+      <c r="C15" s="67" t="n">
+        <v>10</v>
+      </c>
       <c r="D15" s="68" t="n"/>
     </row>
     <row r="16" ht="19.5" customHeight="1" s="55">
@@ -1254,12 +1258,8 @@
           <t>bolo de rolo pequeno</t>
         </is>
       </c>
-      <c r="B16" s="66" t="n">
-        <v>1</v>
-      </c>
-      <c r="C16" s="67" t="n">
-        <v>2</v>
-      </c>
+      <c r="B16" s="66" t="n"/>
+      <c r="C16" s="67" t="n"/>
       <c r="D16" s="68" t="n"/>
     </row>
     <row r="17" ht="19.5" customHeight="1" s="55">
@@ -1268,12 +1268,8 @@
           <t>doce de leite pequeno</t>
         </is>
       </c>
-      <c r="B17" s="66" t="n">
-        <v>7</v>
-      </c>
-      <c r="C17" s="67" t="n">
-        <v>24.5</v>
-      </c>
+      <c r="B17" s="66" t="n"/>
+      <c r="C17" s="67" t="n"/>
       <c r="D17" s="68" t="n"/>
     </row>
     <row r="18" ht="19.5" customHeight="1" s="55">
@@ -1312,12 +1308,8 @@
           <t>nego bom</t>
         </is>
       </c>
-      <c r="B21" s="66" t="n">
-        <v>4</v>
-      </c>
-      <c r="C21" s="67" t="n">
-        <v>40</v>
-      </c>
+      <c r="B21" s="66" t="n"/>
+      <c r="C21" s="67" t="n"/>
       <c r="D21" s="68" t="n"/>
     </row>
     <row r="22" ht="19.5" customHeight="1" s="55">
@@ -1336,12 +1328,8 @@
           <t>beiju recheado</t>
         </is>
       </c>
-      <c r="B23" s="66" t="n">
-        <v>1</v>
-      </c>
-      <c r="C23" s="67" t="n">
-        <v>12</v>
-      </c>
+      <c r="B23" s="66" t="n"/>
+      <c r="C23" s="67" t="n"/>
       <c r="D23" s="68" t="n"/>
     </row>
     <row r="24" ht="19.5" customHeight="1" s="55">
@@ -1351,10 +1339,10 @@
         </is>
       </c>
       <c r="B24" s="66" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C24" s="67" t="n">
-        <v>59.28</v>
+        <v>15</v>
       </c>
       <c r="D24" s="68" t="n"/>
     </row>
@@ -1365,10 +1353,10 @@
         </is>
       </c>
       <c r="B25" s="66" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C25" s="67" t="n">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="D25" s="68" t="n"/>
     </row>
@@ -1378,12 +1366,8 @@
           <t>pingo bel</t>
         </is>
       </c>
-      <c r="B26" s="66" t="n">
-        <v>1</v>
-      </c>
-      <c r="C26" s="67" t="n">
-        <v>3.5</v>
-      </c>
+      <c r="B26" s="66" t="n"/>
+      <c r="C26" s="67" t="n"/>
       <c r="D26" s="68" t="n"/>
     </row>
     <row r="27" ht="19.5" customHeight="1" s="55">
@@ -1425,12 +1409,8 @@
           <t>cocada grande</t>
         </is>
       </c>
-      <c r="B30" s="66" t="n">
-        <v>2</v>
-      </c>
-      <c r="C30" s="67" t="n">
-        <v>20</v>
-      </c>
+      <c r="B30" s="66" t="n"/>
+      <c r="C30" s="67" t="n"/>
       <c r="D30" s="68" t="n"/>
       <c r="E30" s="74" t="n"/>
     </row>
@@ -1441,10 +1421,10 @@
         </is>
       </c>
       <c r="B31" s="66" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C31" s="67" t="n">
-        <v>14</v>
+        <v>3.5</v>
       </c>
       <c r="D31" s="68" t="n"/>
       <c r="E31" s="74" t="n"/>
@@ -1477,8 +1457,12 @@
           <t>coquero</t>
         </is>
       </c>
-      <c r="B34" s="66" t="n"/>
-      <c r="C34" s="67" t="n"/>
+      <c r="B34" s="66" t="n">
+        <v>1</v>
+      </c>
+      <c r="C34" s="67" t="n">
+        <v>3</v>
+      </c>
       <c r="D34" s="68" t="n"/>
       <c r="E34" s="74" t="n"/>
     </row>
@@ -1499,12 +1483,8 @@
           <t>coca</t>
         </is>
       </c>
-      <c r="B36" s="66" t="n">
-        <v>3</v>
-      </c>
-      <c r="C36" s="67" t="n">
-        <v>15</v>
-      </c>
+      <c r="B36" s="66" t="n"/>
+      <c r="C36" s="67" t="n"/>
       <c r="D36" s="68" t="n"/>
     </row>
     <row r="37" ht="19.5" customHeight="1" s="55">
@@ -1564,10 +1544,10 @@
         </is>
       </c>
       <c r="B42" s="66" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C42" s="67" t="n">
-        <v>11.99</v>
+        <v>8.960000000000001</v>
       </c>
       <c r="D42" s="68" t="n"/>
     </row>
@@ -1577,8 +1557,12 @@
           <t>agua c/ gás</t>
         </is>
       </c>
-      <c r="B43" s="66" t="n"/>
-      <c r="C43" s="67" t="n"/>
+      <c r="B43" s="66" t="n">
+        <v>1</v>
+      </c>
+      <c r="C43" s="67" t="n">
+        <v>4</v>
+      </c>
       <c r="D43" s="68" t="n"/>
     </row>
     <row r="44" ht="19.5" customHeight="1" s="55">
@@ -1653,13 +1637,29 @@
       <c r="D50" s="76" t="n"/>
     </row>
     <row r="51" ht="17.25" customHeight="1" s="55">
-      <c r="A51" s="89" t="n"/>
-      <c r="B51" s="67" t="n"/>
+      <c r="A51" s="89" t="inlineStr">
+        <is>
+          <t>OVOS</t>
+        </is>
+      </c>
+      <c r="B51" s="67" t="inlineStr">
+        <is>
+          <t>24,00</t>
+        </is>
+      </c>
       <c r="C51" s="90" t="n"/>
     </row>
     <row r="52" ht="15" customFormat="1" customHeight="1" s="91">
-      <c r="A52" s="92" t="n"/>
-      <c r="B52" s="67" t="n"/>
+      <c r="A52" s="92" t="inlineStr">
+        <is>
+          <t>VASSOURA</t>
+        </is>
+      </c>
+      <c r="B52" s="67" t="inlineStr">
+        <is>
+          <t>30,00</t>
+        </is>
+      </c>
     </row>
     <row r="53" ht="18" customHeight="1" s="55">
       <c r="A53" s="93" t="n"/>
@@ -1713,7 +1713,11 @@
           <t>DINHEIRO</t>
         </is>
       </c>
-      <c r="B60" s="67" t="n"/>
+      <c r="B60" s="67" t="inlineStr">
+        <is>
+          <t>183,00</t>
+        </is>
+      </c>
       <c r="C60" s="101" t="n"/>
     </row>
     <row r="61" ht="18.75" customHeight="1" s="55">
@@ -1722,7 +1726,11 @@
           <t>DEBITO</t>
         </is>
       </c>
-      <c r="B61" s="67" t="n"/>
+      <c r="B61" s="67" t="inlineStr">
+        <is>
+          <t>182,00</t>
+        </is>
+      </c>
       <c r="C61" s="88" t="n"/>
     </row>
     <row r="62" ht="18.75" customHeight="1" s="55">
@@ -1731,7 +1739,11 @@
           <t>PIX</t>
         </is>
       </c>
-      <c r="B62" s="67" t="n"/>
+      <c r="B62" s="67" t="inlineStr">
+        <is>
+          <t>328,00</t>
+        </is>
+      </c>
       <c r="C62" s="88" t="n"/>
     </row>
     <row r="63" ht="18.75" customHeight="1" s="55">

</xml_diff>